<commit_message>
sinalizacao colunas obrig. xlsx
</commit_message>
<xml_diff>
--- a/public/templates/PDV_Template.xlsx
+++ b/public/templates/PDV_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\OneDrive\Área de Trabalho\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A2FDE1C-30D8-4AF9-A84A-7C71279938C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{127DA940-1C56-4FBA-A59D-E6AAD963FDCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{14EB5F34-71E6-4BB0-9F9B-50B59782F13C}"/>
   </bookViews>
@@ -97,12 +97,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -118,11 +124,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -131,12 +137,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -455,7 +463,7 @@
   <dimension ref="A1:J221"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -470,7 +478,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -479,22 +487,22 @@
       <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="9" t="s">
         <v>2</v>
       </c>
       <c r="J1" s="2" t="s">

</xml_diff>